<commit_message>
finished annual rainfed SOC calculations. explored some results which look fine
</commit_message>
<xml_diff>
--- a/data/crops/rothc_support/annual_crops_rothc_scenarios_irrigated.xlsx
+++ b/data/crops/rothc_support/annual_crops_rothc_scenarios_irrigated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/rothc_support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{33C6C299-611E-4211-942E-822619945D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC94AC02-2D58-4CBA-9441-3FD2E0379EEC}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{33C6C299-611E-4211-942E-822619945D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4F97AC3-D3B0-4BE1-A2F3-6D6C34B624D3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F94B64D-243B-49DA-AE87-045B34BFAB0F}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2132" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="482">
   <si>
     <t>crop_name</t>
   </si>
@@ -1485,6 +1485,9 @@
   </si>
   <si>
     <t>practices_string_id</t>
+  </si>
+  <si>
+    <t>force_new_file</t>
   </si>
 </sst>
 </file>
@@ -1537,9 +1540,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1874,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1821CC5-2977-4A1A-B60B-8C004F05C4AF}">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1891,69 +1895,72 @@
     <col min="8" max="8" width="63.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U1" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2009,8 +2016,11 @@
       <c r="T2" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2066,8 +2076,11 @@
       <c r="T3" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2123,8 +2136,11 @@
       <c r="T4" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2180,8 +2196,11 @@
       <c r="T5" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2237,8 +2256,11 @@
       <c r="T6" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2294,8 +2316,11 @@
       <c r="T7" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2351,8 +2376,11 @@
       <c r="T8" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2408,8 +2436,11 @@
       <c r="T9" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2465,8 +2496,11 @@
       <c r="T10" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2522,8 +2556,11 @@
       <c r="T11" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2579,8 +2616,11 @@
       <c r="T12" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2636,8 +2676,11 @@
       <c r="T13" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2693,8 +2736,11 @@
       <c r="T14" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2750,8 +2796,11 @@
       <c r="T15" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2807,8 +2856,11 @@
       <c r="T16" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -2864,8 +2916,11 @@
       <c r="T17" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2921,8 +2976,11 @@
       <c r="T18" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2978,8 +3036,11 @@
       <c r="T19" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -3035,8 +3096,11 @@
       <c r="T20" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -3092,8 +3156,11 @@
       <c r="T21" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3149,8 +3216,11 @@
       <c r="T22" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -3206,8 +3276,11 @@
       <c r="T23" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="U23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -3262,6 +3335,9 @@
       </c>
       <c r="T24" t="s">
         <v>458</v>
+      </c>
+      <c r="U24" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculated all SOC LEAFs raster for conservation tillage
</commit_message>
<xml_diff>
--- a/data/crops/rothc_support/annual_crops_rothc_scenarios_irrigated.xlsx
+++ b/data/crops/rothc_support/annual_crops_rothc_scenarios_irrigated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/cristobal_loyola_wwfus_org/Documents/Documents/203. Python projects/SBTN_Test/data/crops/rothc_support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{33C6C299-611E-4211-942E-822619945D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4F97AC3-D3B0-4BE1-A2F3-6D6C34B624D3}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{33C6C299-611E-4211-942E-822619945D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFE7A3E1-B7C2-4903-B2C4-0F8C6205368F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6F94B64D-243B-49DA-AE87-045B34BFAB0F}"/>
   </bookViews>
@@ -1880,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1821CC5-2977-4A1A-B60B-8C004F05C4AF}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="I5" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>